<commit_message>
修复 ILRuntime try中return 无catch finally中代码不执行的问题
</commit_message>
<xml_diff>
--- a/Excel/C_ServerConfig.xlsx
+++ b/Excel/C_ServerConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitProject\ET_Framwork\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19D3B04-C25E-406F-9953-E995B99F2F62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5F1CD4-EF01-4292-A3C1-702DF13F97F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -130,6 +130,14 @@
   </si>
   <si>
     <t>http://172.22.213.58:8081/cdn_test</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否默认值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsPriority</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -521,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:K7"/>
+  <dimension ref="C2:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -543,12 +551,12 @@
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
@@ -576,8 +584,11 @@
       <c r="K3" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="L3" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
@@ -603,8 +614,11 @@
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
@@ -630,8 +644,11 @@
       <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="L5" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="3:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -659,8 +676,11 @@
       <c r="K6" s="5">
         <v>1</v>
       </c>
+      <c r="L6" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -687,6 +707,9 @@
       </c>
       <c r="K7" s="5">
         <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>